<commit_message>
feat: :sparkles: upload students and inser parents
</commit_message>
<xml_diff>
--- a/students.xlsx
+++ b/students.xlsx
@@ -11,7 +11,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="36" uniqueCount="33">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="132" uniqueCount="111">
   <si>
     <t>firstName</t>
   </si>
@@ -31,85 +31,319 @@
     <t>phoneNumber2</t>
   </si>
   <si>
-    <t>parentId</t>
+    <t>parentName</t>
+  </si>
+  <si>
+    <t>parentLastName</t>
+  </si>
+  <si>
+    <t>parentAddress</t>
+  </si>
+  <si>
+    <t>parentNumber1</t>
+  </si>
+  <si>
+    <t>parentTc</t>
   </si>
   <si>
     <t>institutionKey</t>
   </si>
   <si>
-    <t>John</t>
-  </si>
-  <si>
-    <t>Doe</t>
+    <t>Ahmet</t>
+  </si>
+  <si>
+    <t>Yılmaz</t>
   </si>
   <si>
     <t>12345678901</t>
   </si>
   <si>
-    <t>123 Main St, Springfield</t>
-  </si>
-  <si>
-    <t>555-1234</t>
-  </si>
-  <si>
-    <t>555-5678</t>
-  </si>
-  <si>
-    <t>INST-KEY-001</t>
-  </si>
-  <si>
-    <t>Jane</t>
-  </si>
-  <si>
-    <t>Smith</t>
+    <t>İstanbul, Kadıköy</t>
+  </si>
+  <si>
+    <t>05001234567</t>
+  </si>
+  <si>
+    <t>05007654321</t>
+  </si>
+  <si>
+    <t>Mehmet</t>
+  </si>
+  <si>
+    <t>Ankara, Çankaya</t>
+  </si>
+  <si>
+    <t>03121234567</t>
+  </si>
+  <si>
+    <t>10987654321</t>
+  </si>
+  <si>
+    <t>INST001</t>
+  </si>
+  <si>
+    <t>Ayşe</t>
+  </si>
+  <si>
+    <t>Demir</t>
   </si>
   <si>
     <t>23456789012</t>
   </si>
   <si>
-    <t>456 Oak St, Springfield</t>
-  </si>
-  <si>
-    <t>555-2345</t>
-  </si>
-  <si>
-    <t>555-6789</t>
-  </si>
-  <si>
-    <t>Alice</t>
-  </si>
-  <si>
-    <t>Johnson</t>
+    <t>İzmir, Karşıyaka</t>
+  </si>
+  <si>
+    <t>05009876543</t>
+  </si>
+  <si>
+    <t/>
+  </si>
+  <si>
+    <t>Fatma</t>
+  </si>
+  <si>
+    <t>İzmir, Bornova</t>
+  </si>
+  <si>
+    <t>02324567890</t>
+  </si>
+  <si>
+    <t>19876543210</t>
+  </si>
+  <si>
+    <t>INST002</t>
+  </si>
+  <si>
+    <t>Ali</t>
+  </si>
+  <si>
+    <t>Kaya</t>
   </si>
   <si>
     <t>34567890123</t>
   </si>
   <si>
-    <t>789 Pine St, Springfield</t>
-  </si>
-  <si>
-    <t>555-3456</t>
-  </si>
-  <si>
-    <t>555-7890</t>
-  </si>
-  <si>
-    <t>Bob</t>
-  </si>
-  <si>
-    <t>Williams</t>
+    <t>Bursa, Osmangazi</t>
+  </si>
+  <si>
+    <t>05001112233</t>
+  </si>
+  <si>
+    <t>05004445566</t>
+  </si>
+  <si>
+    <t>Hasan</t>
+  </si>
+  <si>
+    <t>Bursa, Nilüfer</t>
+  </si>
+  <si>
+    <t>02242223344</t>
+  </si>
+  <si>
+    <t>18765432109</t>
+  </si>
+  <si>
+    <t>INST003</t>
+  </si>
+  <si>
+    <t>Zeynep</t>
+  </si>
+  <si>
+    <t>Çelik</t>
   </si>
   <si>
     <t>45678901234</t>
   </si>
   <si>
-    <t>101 Maple Ave, Springfield</t>
-  </si>
-  <si>
-    <t>555-4567</t>
-  </si>
-  <si>
-    <t>555-8901</t>
+    <t>Antalya, Muratpaşa</t>
+  </si>
+  <si>
+    <t>05002223344</t>
+  </si>
+  <si>
+    <t>Emine</t>
+  </si>
+  <si>
+    <t>Antalya, Konyaaltı</t>
+  </si>
+  <si>
+    <t>02423214567</t>
+  </si>
+  <si>
+    <t>17654321098</t>
+  </si>
+  <si>
+    <t>INST004</t>
+  </si>
+  <si>
+    <t>Mert</t>
+  </si>
+  <si>
+    <t>Şahin</t>
+  </si>
+  <si>
+    <t>56789012345</t>
+  </si>
+  <si>
+    <t>Adana, Seyhan</t>
+  </si>
+  <si>
+    <t>05003334455</t>
+  </si>
+  <si>
+    <t>05006667788</t>
+  </si>
+  <si>
+    <t>Sibel</t>
+  </si>
+  <si>
+    <t>Adana, Yüreğir</t>
+  </si>
+  <si>
+    <t>03222121212</t>
+  </si>
+  <si>
+    <t>16543210987</t>
+  </si>
+  <si>
+    <t>INST005</t>
+  </si>
+  <si>
+    <t>Elif</t>
+  </si>
+  <si>
+    <t>Aydın</t>
+  </si>
+  <si>
+    <t>67890123456</t>
+  </si>
+  <si>
+    <t>Eskişehir, Tepebaşı</t>
+  </si>
+  <si>
+    <t>Zehra</t>
+  </si>
+  <si>
+    <t>Eskişehir, Odunpazarı</t>
+  </si>
+  <si>
+    <t>02223334455</t>
+  </si>
+  <si>
+    <t>15432109876</t>
+  </si>
+  <si>
+    <t>INST006</t>
+  </si>
+  <si>
+    <t>Can</t>
+  </si>
+  <si>
+    <t>Güneş</t>
+  </si>
+  <si>
+    <t>78901234567</t>
+  </si>
+  <si>
+    <t>Konya, Selçuklu</t>
+  </si>
+  <si>
+    <t>05005556677</t>
+  </si>
+  <si>
+    <t>05008889900</t>
+  </si>
+  <si>
+    <t>Konya, Meram</t>
+  </si>
+  <si>
+    <t>03324324324</t>
+  </si>
+  <si>
+    <t>14321098765</t>
+  </si>
+  <si>
+    <t>INST007</t>
+  </si>
+  <si>
+    <t>Derya</t>
+  </si>
+  <si>
+    <t>Koç</t>
+  </si>
+  <si>
+    <t>89012345678</t>
+  </si>
+  <si>
+    <t>Samsun, Atakum</t>
+  </si>
+  <si>
+    <t>Selma</t>
+  </si>
+  <si>
+    <t>Samsun, İlkadım</t>
+  </si>
+  <si>
+    <t>03622334455</t>
+  </si>
+  <si>
+    <t>13210987654</t>
+  </si>
+  <si>
+    <t>INST008</t>
+  </si>
+  <si>
+    <t>Emre</t>
+  </si>
+  <si>
+    <t>Polat</t>
+  </si>
+  <si>
+    <t>90123456789</t>
+  </si>
+  <si>
+    <t>Trabzon, Ortahisar</t>
+  </si>
+  <si>
+    <t>05007778899</t>
+  </si>
+  <si>
+    <t>Murat</t>
+  </si>
+  <si>
+    <t>Trabzon, Yomra</t>
+  </si>
+  <si>
+    <t>04622334455</t>
+  </si>
+  <si>
+    <t>12109876543</t>
+  </si>
+  <si>
+    <t>INST009</t>
+  </si>
+  <si>
+    <t>Yıldız</t>
+  </si>
+  <si>
+    <t>01234567890</t>
+  </si>
+  <si>
+    <t>Gaziantep, Şahinbey</t>
+  </si>
+  <si>
+    <t>Gaziantep, Şehitkamil</t>
+  </si>
+  <si>
+    <t>03424445566</t>
+  </si>
+  <si>
+    <t>11098765432</t>
+  </si>
+  <si>
+    <t>INST010</t>
   </si>
 </sst>
 </file>
@@ -486,17 +720,17 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:H5"/>
+  <dimension ref="A1:L11"/>
   <sheetFormatPr defaultRowHeight="15" outlineLevelRow="0" outlineLevelCol="0" x14ac:dyDescent="55"/>
   <cols>
     <col min="1" max="3" width="15" customWidth="1"/>
     <col min="4" max="4" width="30" customWidth="1"/>
     <col min="5" max="6" width="15" customWidth="1"/>
-    <col min="7" max="7" width="10" customWidth="1"/>
-    <col min="8" max="8" width="20" customWidth="1"/>
+    <col min="7" max="11" width="10" customWidth="1"/>
+    <col min="12" max="12" width="20" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -521,109 +755,397 @@
       <c r="H1" t="s">
         <v>7</v>
       </c>
+      <c r="I1" t="s">
+        <v>8</v>
+      </c>
+      <c r="J1" t="s">
+        <v>9</v>
+      </c>
+      <c r="K1" t="s">
+        <v>10</v>
+      </c>
+      <c r="L1" t="s">
+        <v>11</v>
+      </c>
     </row>
-    <row r="2" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>8</v>
+        <v>12</v>
       </c>
       <c r="B2" t="s">
-        <v>9</v>
+        <v>13</v>
       </c>
       <c r="C2" t="s">
-        <v>10</v>
+        <v>14</v>
       </c>
       <c r="D2" t="s">
-        <v>11</v>
+        <v>15</v>
       </c>
       <c r="E2" t="s">
+        <v>16</v>
+      </c>
+      <c r="F2" t="s">
+        <v>17</v>
+      </c>
+      <c r="G2" t="s">
+        <v>18</v>
+      </c>
+      <c r="H2" t="s">
+        <v>13</v>
+      </c>
+      <c r="I2" t="s">
+        <v>19</v>
+      </c>
+      <c r="J2" t="s">
+        <v>20</v>
+      </c>
+      <c r="K2" t="s">
+        <v>21</v>
+      </c>
+      <c r="L2" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="3" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>23</v>
+      </c>
+      <c r="B3" t="s">
+        <v>24</v>
+      </c>
+      <c r="C3" t="s">
+        <v>25</v>
+      </c>
+      <c r="D3" t="s">
+        <v>26</v>
+      </c>
+      <c r="E3" t="s">
+        <v>27</v>
+      </c>
+      <c r="F3" t="s">
+        <v>28</v>
+      </c>
+      <c r="G3" t="s">
+        <v>29</v>
+      </c>
+      <c r="H3" t="s">
+        <v>24</v>
+      </c>
+      <c r="I3" t="s">
+        <v>30</v>
+      </c>
+      <c r="J3" t="s">
+        <v>31</v>
+      </c>
+      <c r="K3" t="s">
+        <v>32</v>
+      </c>
+      <c r="L3" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="4" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>34</v>
+      </c>
+      <c r="B4" t="s">
+        <v>35</v>
+      </c>
+      <c r="C4" t="s">
+        <v>36</v>
+      </c>
+      <c r="D4" t="s">
+        <v>37</v>
+      </c>
+      <c r="E4" t="s">
+        <v>38</v>
+      </c>
+      <c r="F4" t="s">
+        <v>39</v>
+      </c>
+      <c r="G4" t="s">
+        <v>40</v>
+      </c>
+      <c r="H4" t="s">
+        <v>35</v>
+      </c>
+      <c r="I4" t="s">
+        <v>41</v>
+      </c>
+      <c r="J4" t="s">
+        <v>42</v>
+      </c>
+      <c r="K4" t="s">
+        <v>43</v>
+      </c>
+      <c r="L4" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="5" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>45</v>
+      </c>
+      <c r="B5" t="s">
+        <v>46</v>
+      </c>
+      <c r="C5" t="s">
+        <v>47</v>
+      </c>
+      <c r="D5" t="s">
+        <v>48</v>
+      </c>
+      <c r="E5" t="s">
+        <v>49</v>
+      </c>
+      <c r="F5" t="s">
+        <v>28</v>
+      </c>
+      <c r="G5" t="s">
+        <v>50</v>
+      </c>
+      <c r="H5" t="s">
+        <v>46</v>
+      </c>
+      <c r="I5" t="s">
+        <v>51</v>
+      </c>
+      <c r="J5" t="s">
+        <v>52</v>
+      </c>
+      <c r="K5" t="s">
+        <v>53</v>
+      </c>
+      <c r="L5" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="6" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>55</v>
+      </c>
+      <c r="B6" t="s">
+        <v>56</v>
+      </c>
+      <c r="C6" t="s">
+        <v>57</v>
+      </c>
+      <c r="D6" t="s">
+        <v>58</v>
+      </c>
+      <c r="E6" t="s">
+        <v>59</v>
+      </c>
+      <c r="F6" t="s">
+        <v>60</v>
+      </c>
+      <c r="G6" t="s">
+        <v>61</v>
+      </c>
+      <c r="H6" t="s">
+        <v>56</v>
+      </c>
+      <c r="I6" t="s">
+        <v>62</v>
+      </c>
+      <c r="J6" t="s">
+        <v>63</v>
+      </c>
+      <c r="K6" t="s">
+        <v>64</v>
+      </c>
+      <c r="L6" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="7" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
+        <v>66</v>
+      </c>
+      <c r="B7" t="s">
+        <v>67</v>
+      </c>
+      <c r="C7" t="s">
+        <v>68</v>
+      </c>
+      <c r="D7" t="s">
+        <v>69</v>
+      </c>
+      <c r="E7" t="s">
+        <v>39</v>
+      </c>
+      <c r="F7" t="s">
+        <v>28</v>
+      </c>
+      <c r="G7" t="s">
+        <v>70</v>
+      </c>
+      <c r="H7" t="s">
+        <v>67</v>
+      </c>
+      <c r="I7" t="s">
+        <v>71</v>
+      </c>
+      <c r="J7" t="s">
+        <v>72</v>
+      </c>
+      <c r="K7" t="s">
+        <v>73</v>
+      </c>
+      <c r="L7" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="8" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A8" t="s">
+        <v>75</v>
+      </c>
+      <c r="B8" t="s">
+        <v>76</v>
+      </c>
+      <c r="C8" t="s">
+        <v>77</v>
+      </c>
+      <c r="D8" t="s">
+        <v>78</v>
+      </c>
+      <c r="E8" t="s">
+        <v>79</v>
+      </c>
+      <c r="F8" t="s">
+        <v>80</v>
+      </c>
+      <c r="G8" t="s">
+        <v>34</v>
+      </c>
+      <c r="H8" t="s">
+        <v>76</v>
+      </c>
+      <c r="I8" t="s">
+        <v>81</v>
+      </c>
+      <c r="J8" t="s">
+        <v>82</v>
+      </c>
+      <c r="K8" t="s">
+        <v>83</v>
+      </c>
+      <c r="L8" t="s">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="9" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A9" t="s">
+        <v>85</v>
+      </c>
+      <c r="B9" t="s">
+        <v>86</v>
+      </c>
+      <c r="C9" t="s">
+        <v>87</v>
+      </c>
+      <c r="D9" t="s">
+        <v>88</v>
+      </c>
+      <c r="E9" t="s">
+        <v>60</v>
+      </c>
+      <c r="F9" t="s">
+        <v>28</v>
+      </c>
+      <c r="G9" t="s">
+        <v>89</v>
+      </c>
+      <c r="H9" t="s">
+        <v>86</v>
+      </c>
+      <c r="I9" t="s">
+        <v>90</v>
+      </c>
+      <c r="J9" t="s">
+        <v>91</v>
+      </c>
+      <c r="K9" t="s">
+        <v>92</v>
+      </c>
+      <c r="L9" t="s">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="10" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A10" t="s">
+        <v>94</v>
+      </c>
+      <c r="B10" t="s">
+        <v>95</v>
+      </c>
+      <c r="C10" t="s">
+        <v>96</v>
+      </c>
+      <c r="D10" t="s">
+        <v>97</v>
+      </c>
+      <c r="E10" t="s">
+        <v>98</v>
+      </c>
+      <c r="F10" t="s">
+        <v>38</v>
+      </c>
+      <c r="G10" t="s">
+        <v>99</v>
+      </c>
+      <c r="H10" t="s">
+        <v>95</v>
+      </c>
+      <c r="I10" t="s">
+        <v>100</v>
+      </c>
+      <c r="J10" t="s">
+        <v>101</v>
+      </c>
+      <c r="K10" t="s">
+        <v>102</v>
+      </c>
+      <c r="L10" t="s">
+        <v>103</v>
+      </c>
+    </row>
+    <row r="11" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A11" t="s">
+        <v>29</v>
+      </c>
+      <c r="B11" t="s">
+        <v>104</v>
+      </c>
+      <c r="C11" t="s">
+        <v>105</v>
+      </c>
+      <c r="D11" t="s">
+        <v>106</v>
+      </c>
+      <c r="E11" t="s">
+        <v>80</v>
+      </c>
+      <c r="F11" t="s">
+        <v>28</v>
+      </c>
+      <c r="G11" t="s">
         <v>12</v>
       </c>
-      <c r="F2" t="s">
-        <v>13</v>
-      </c>
-      <c r="G2">
-        <v>1</v>
-      </c>
-      <c r="H2" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="3" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A3" t="s">
-        <v>15</v>
-      </c>
-      <c r="B3" t="s">
-        <v>16</v>
-      </c>
-      <c r="C3" t="s">
-        <v>17</v>
-      </c>
-      <c r="D3" t="s">
-        <v>18</v>
-      </c>
-      <c r="E3" t="s">
-        <v>19</v>
-      </c>
-      <c r="F3" t="s">
-        <v>20</v>
-      </c>
-      <c r="G3">
-        <v>2</v>
-      </c>
-      <c r="H3" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="4" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A4" t="s">
-        <v>21</v>
-      </c>
-      <c r="B4" t="s">
-        <v>22</v>
-      </c>
-      <c r="C4" t="s">
-        <v>23</v>
-      </c>
-      <c r="D4" t="s">
-        <v>24</v>
-      </c>
-      <c r="E4" t="s">
-        <v>25</v>
-      </c>
-      <c r="F4" t="s">
-        <v>26</v>
-      </c>
-      <c r="G4">
-        <v>3</v>
-      </c>
-      <c r="H4" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="5" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A5" t="s">
-        <v>27</v>
-      </c>
-      <c r="B5" t="s">
-        <v>28</v>
-      </c>
-      <c r="C5" t="s">
-        <v>29</v>
-      </c>
-      <c r="D5" t="s">
-        <v>30</v>
-      </c>
-      <c r="E5" t="s">
-        <v>31</v>
-      </c>
-      <c r="F5" t="s">
-        <v>32</v>
-      </c>
-      <c r="G5">
-        <v>4</v>
-      </c>
-      <c r="H5" t="s">
-        <v>14</v>
+      <c r="H11" t="s">
+        <v>104</v>
+      </c>
+      <c r="I11" t="s">
+        <v>107</v>
+      </c>
+      <c r="J11" t="s">
+        <v>108</v>
+      </c>
+      <c r="K11" t="s">
+        <v>109</v>
+      </c>
+      <c r="L11" t="s">
+        <v>110</v>
       </c>
     </row>
   </sheetData>

</xml_diff>